<commit_message>
Support NMVOC point sources, use cache for flanders spatial pattern data
</commit_message>
<xml_diff>
--- a/logic/test/data/spatialinventory/bef/reporting_2021/2015/Emissies per km2 excl puntbrongegevens_2015_NOx.xlsx
+++ b/logic/test/data/spatialinventory/bef/reporting_2021/2015/Emissies per km2 excl puntbrongegevens_2015_NOx.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\spatialinventory\bef\reporting_2021\2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E03394E-C61B-4019-88EF-33393E7748ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B24725A-6F50-44D3-936E-6909765662A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4400" yWindow="9290" windowWidth="27040" windowHeight="10780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2019_PM2.5" sheetId="1" r:id="rId1"/>
+    <sheet name="2019_NOx" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2019_PM2.5'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2019_NOx'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -54,10 +54,10 @@
     <t>1A2a</t>
   </si>
   <si>
-    <t>PM2,5</t>
-  </si>
-  <si>
     <t>t/jr</t>
+  </si>
+  <si>
+    <t>NOx</t>
   </si>
 </sst>
 </file>
@@ -387,17 +387,17 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="1" max="5" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="20.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -428,7 +428,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>38000</v>
@@ -440,7 +440,7 @@
         <v>2.8531966276199998E-4</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>